<commit_message>
Cosmetic changes to reports.
</commit_message>
<xml_diff>
--- a/misc/Requests.xlsx
+++ b/misc/Requests.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Requests" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Priortiy</t>
   </si>
@@ -30,15 +30,9 @@
     <t>Estimated Completion Date</t>
   </si>
   <si>
-    <t>High</t>
-  </si>
-  <si>
     <t>Stock Control System Requests</t>
   </si>
   <si>
-    <t>Dispatch note changes for new automated system</t>
-  </si>
-  <si>
     <t>Low</t>
   </si>
   <si>
@@ -54,19 +48,28 @@
     <t>Create a 'Reports' section to declutter 'Products'</t>
   </si>
   <si>
-    <t>September</t>
-  </si>
-  <si>
     <t>Merge 'add' functionality to products + customers section</t>
   </si>
   <si>
-    <t xml:space="preserve">Use a template excel sheet </t>
+    <t>Products PO stock split per order + date</t>
+  </si>
+  <si>
+    <t>Alert when selecting customer for a new order</t>
+  </si>
+  <si>
+    <t>Proforma customer alert</t>
+  </si>
+  <si>
+    <t>Use a template excel sheet for each report</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -261,24 +264,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -288,17 +291,24 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="8">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -628,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E34"/>
+  <dimension ref="B1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -642,230 +652,226 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="18">
-      <c r="B1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="B1" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="2:5" ht="16" thickBot="1"/>
     <row r="3" spans="2:5" ht="19" thickBot="1">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="2:5">
-      <c r="B4" s="12" t="s">
+      <c r="D4" s="17">
+        <v>42641</v>
+      </c>
+      <c r="E4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="13" t="s">
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="19">
+        <v>42650</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="18">
-        <v>42641</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="D6" s="19">
+        <v>42653</v>
+      </c>
+      <c r="E6" s="14"/>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="16"/>
-    </row>
-    <row r="6" spans="2:5">
-      <c r="B6" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="19">
-        <v>42645</v>
-      </c>
-      <c r="E6" s="16" t="s">
+      <c r="D7" s="18">
+        <v>42660</v>
+      </c>
+      <c r="E7" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="6"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="16"/>
-    </row>
     <row r="8" spans="2:5">
-      <c r="B8" s="6"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="16"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="14"/>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="6"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="16"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="14"/>
     </row>
     <row r="10" spans="2:5">
-      <c r="B10" s="6"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="16"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="14"/>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="6"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="16"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="14"/>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="6"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="16"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="14"/>
     </row>
     <row r="13" spans="2:5">
-      <c r="B13" s="6"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="16"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="14"/>
     </row>
     <row r="14" spans="2:5">
-      <c r="B14" s="6"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="16"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="14"/>
     </row>
     <row r="15" spans="2:5">
-      <c r="B15" s="6"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="16"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="14"/>
     </row>
     <row r="16" spans="2:5">
-      <c r="B16" s="6"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="16"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="14"/>
     </row>
     <row r="17" spans="2:5">
-      <c r="B17" s="6"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="16"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="14"/>
     </row>
     <row r="18" spans="2:5">
-      <c r="B18" s="6"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="16"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="14"/>
     </row>
     <row r="19" spans="2:5">
-      <c r="B19" s="6"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="16"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="14"/>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="6"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="16"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="14"/>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="6"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="16"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="14"/>
     </row>
     <row r="22" spans="2:5">
-      <c r="B22" s="6"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="16"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="14"/>
     </row>
     <row r="23" spans="2:5">
-      <c r="B23" s="6"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="16"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="14"/>
     </row>
     <row r="24" spans="2:5">
-      <c r="B24" s="6"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="16"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="14"/>
     </row>
     <row r="25" spans="2:5">
-      <c r="B25" s="6"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="16"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="14"/>
     </row>
     <row r="26" spans="2:5">
-      <c r="B26" s="6"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="16"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="14"/>
     </row>
     <row r="27" spans="2:5">
-      <c r="B27" s="6"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="16"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="14"/>
     </row>
     <row r="28" spans="2:5">
-      <c r="B28" s="6"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="16"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="14"/>
     </row>
     <row r="29" spans="2:5">
-      <c r="B29" s="6"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="16"/>
-    </row>
-    <row r="30" spans="2:5">
+      <c r="B29" s="5"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="14"/>
+    </row>
+    <row r="30" spans="2:5" ht="16" thickBot="1">
       <c r="B30" s="6"/>
       <c r="C30" s="4"/>
       <c r="D30" s="20"/>
-      <c r="E30" s="16"/>
+      <c r="E30" s="15"/>
     </row>
     <row r="31" spans="2:5">
-      <c r="B31" s="6"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="16"/>
-    </row>
-    <row r="32" spans="2:5" ht="16" thickBot="1">
-      <c r="B32" s="7"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="17"/>
-    </row>
-    <row r="33" spans="2:4">
-      <c r="B33" s="1"/>
-      <c r="D33" s="2"/>
-    </row>
-    <row r="34" spans="2:4">
-      <c r="B34" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="2:5">
+      <c r="B32" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Main change is using templates for reports.
</commit_message>
<xml_diff>
--- a/misc/Requests.xlsx
+++ b/misc/Requests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Requests" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Priortiy</t>
   </si>
@@ -61,6 +61,18 @@
   </si>
   <si>
     <t>Use a template excel sheet for each report</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Update quantity of product when editing sales order</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Incorrect warehouse stock count on 'Products' screen</t>
   </si>
 </sst>
 </file>
@@ -129,7 +141,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -257,8 +269,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -267,8 +288,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -280,31 +303,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="10">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -648,12 +675,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="18">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="2:5" ht="16" thickBot="1"/>
     <row r="3" spans="2:5" ht="19" thickBot="1">
@@ -674,193 +701,205 @@
       <c r="B4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="17">
         <v>42641</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="18" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="17">
         <v>42650</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="18" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="17">
         <v>42653</v>
       </c>
-      <c r="E6" s="12"/>
+      <c r="E6" s="18"/>
     </row>
     <row r="7" spans="2:5">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="22">
         <v>42660</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:5">
-      <c r="B8" s="5"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="12"/>
+      <c r="B8" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="24">
+        <v>42660</v>
+      </c>
+      <c r="E8" s="18"/>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="5"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="12"/>
+      <c r="B9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="11"/>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="5"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="12"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="11"/>
     </row>
     <row r="11" spans="2:5">
       <c r="B11" s="5"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="12"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="11"/>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="5"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="12"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="11"/>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="5"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="12"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="11"/>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" s="5"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="12"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="11"/>
     </row>
     <row r="15" spans="2:5">
       <c r="B15" s="5"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="12"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="11"/>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" s="5"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="12"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="11"/>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="5"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="12"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="11"/>
     </row>
     <row r="18" spans="2:5">
       <c r="B18" s="5"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="12"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="11"/>
     </row>
     <row r="19" spans="2:5">
       <c r="B19" s="5"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="12"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="11"/>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" s="5"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="12"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="11"/>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="5"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="12"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="11"/>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" s="5"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="12"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="11"/>
     </row>
     <row r="23" spans="2:5">
       <c r="B23" s="5"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="12"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="11"/>
     </row>
     <row r="24" spans="2:5">
       <c r="B24" s="5"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="12"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="11"/>
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="5"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="12"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="11"/>
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="5"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="12"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="11"/>
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="5"/>
       <c r="C27" s="3"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="12"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="11"/>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="5"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="12"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="11"/>
     </row>
     <row r="29" spans="2:5">
       <c r="B29" s="5"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="12"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="11"/>
     </row>
     <row r="30" spans="2:5" ht="16" thickBot="1">
       <c r="B30" s="6"/>
       <c r="C30" s="4"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="13"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="12"/>
     </row>
     <row r="31" spans="2:5">
       <c r="B31" s="1"/>

</xml_diff>

<commit_message>
Dispatch note alterations for new warehouse.
</commit_message>
<xml_diff>
--- a/misc/Requests.xlsx
+++ b/misc/Requests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="29780" windowHeight="17620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Requests" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>Priortiy</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>Incorrect warehouse stock count on 'Products' screen</t>
+  </si>
+  <si>
+    <t>Dispatch note alterations for new warehouse</t>
+  </si>
+  <si>
+    <t>Time Spent</t>
+  </si>
+  <si>
+    <t>2h</t>
   </si>
 </sst>
 </file>
@@ -279,9 +288,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -312,26 +325,30 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="14">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -661,29 +678,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E32"/>
+  <dimension ref="B1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1"/>
+      <selection activeCell="B1" sqref="B1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="58.33203125" customWidth="1"/>
     <col min="4" max="4" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.1640625" customWidth="1"/>
+    <col min="5" max="5" width="48.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="18">
-      <c r="B1" s="20" t="s">
+    <row r="1" spans="2:6" ht="18">
+      <c r="B1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-    </row>
-    <row r="2" spans="2:5" ht="16" thickBot="1"/>
-    <row r="3" spans="2:5" ht="19" thickBot="1">
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+    </row>
+    <row r="2" spans="2:6" ht="16" thickBot="1"/>
+    <row r="3" spans="2:6" ht="19" thickBot="1">
       <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
@@ -696,8 +715,11 @@
       <c r="E3" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="2:5">
+      <c r="F3" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
       <c r="B4" s="10" t="s">
         <v>7</v>
       </c>
@@ -710,8 +732,11 @@
       <c r="E4" s="18" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="2:5">
+      <c r="F4" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
       <c r="B5" s="15" t="s">
         <v>7</v>
       </c>
@@ -724,8 +749,11 @@
       <c r="E5" s="18" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="2:5">
+      <c r="F5" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
       <c r="B6" s="15" t="s">
         <v>7</v>
       </c>
@@ -736,181 +764,228 @@
         <v>42653</v>
       </c>
       <c r="E6" s="18"/>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="21" t="s">
+      <c r="F6" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="20" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="21">
         <v>42660</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="2:5">
+      <c r="F7" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
       <c r="B8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="23">
         <v>42660</v>
       </c>
       <c r="E8" s="18"/>
-    </row>
-    <row r="9" spans="2:5">
-      <c r="B9" s="5" t="s">
+      <c r="F8" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="23">
+        <v>42688</v>
+      </c>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D10" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="11"/>
-    </row>
-    <row r="10" spans="2:5">
-      <c r="B10" s="5"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="13"/>
       <c r="E10" s="11"/>
-    </row>
-    <row r="11" spans="2:5">
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="2:6">
       <c r="B11" s="5"/>
       <c r="C11" s="3"/>
       <c r="D11" s="13"/>
       <c r="E11" s="11"/>
-    </row>
-    <row r="12" spans="2:5">
+      <c r="F11" s="11"/>
+    </row>
+    <row r="12" spans="2:6">
       <c r="B12" s="5"/>
       <c r="C12" s="3"/>
       <c r="D12" s="13"/>
       <c r="E12" s="11"/>
-    </row>
-    <row r="13" spans="2:5">
+      <c r="F12" s="11"/>
+    </row>
+    <row r="13" spans="2:6">
       <c r="B13" s="5"/>
       <c r="C13" s="3"/>
       <c r="D13" s="13"/>
       <c r="E13" s="11"/>
-    </row>
-    <row r="14" spans="2:5">
+      <c r="F13" s="11"/>
+    </row>
+    <row r="14" spans="2:6">
       <c r="B14" s="5"/>
       <c r="C14" s="3"/>
       <c r="D14" s="13"/>
       <c r="E14" s="11"/>
-    </row>
-    <row r="15" spans="2:5">
+      <c r="F14" s="11"/>
+    </row>
+    <row r="15" spans="2:6">
       <c r="B15" s="5"/>
       <c r="C15" s="3"/>
       <c r="D15" s="13"/>
       <c r="E15" s="11"/>
-    </row>
-    <row r="16" spans="2:5">
+      <c r="F15" s="11"/>
+    </row>
+    <row r="16" spans="2:6">
       <c r="B16" s="5"/>
       <c r="C16" s="3"/>
       <c r="D16" s="13"/>
       <c r="E16" s="11"/>
-    </row>
-    <row r="17" spans="2:5">
+      <c r="F16" s="11"/>
+    </row>
+    <row r="17" spans="2:6">
       <c r="B17" s="5"/>
       <c r="C17" s="3"/>
       <c r="D17" s="13"/>
       <c r="E17" s="11"/>
-    </row>
-    <row r="18" spans="2:5">
+      <c r="F17" s="11"/>
+    </row>
+    <row r="18" spans="2:6">
       <c r="B18" s="5"/>
       <c r="C18" s="3"/>
       <c r="D18" s="13"/>
       <c r="E18" s="11"/>
-    </row>
-    <row r="19" spans="2:5">
+      <c r="F18" s="11"/>
+    </row>
+    <row r="19" spans="2:6">
       <c r="B19" s="5"/>
       <c r="C19" s="3"/>
       <c r="D19" s="13"/>
       <c r="E19" s="11"/>
-    </row>
-    <row r="20" spans="2:5">
+      <c r="F19" s="11"/>
+    </row>
+    <row r="20" spans="2:6">
       <c r="B20" s="5"/>
       <c r="C20" s="3"/>
       <c r="D20" s="13"/>
       <c r="E20" s="11"/>
-    </row>
-    <row r="21" spans="2:5">
+      <c r="F20" s="11"/>
+    </row>
+    <row r="21" spans="2:6">
       <c r="B21" s="5"/>
       <c r="C21" s="3"/>
       <c r="D21" s="13"/>
       <c r="E21" s="11"/>
-    </row>
-    <row r="22" spans="2:5">
+      <c r="F21" s="11"/>
+    </row>
+    <row r="22" spans="2:6">
       <c r="B22" s="5"/>
       <c r="C22" s="3"/>
       <c r="D22" s="13"/>
       <c r="E22" s="11"/>
-    </row>
-    <row r="23" spans="2:5">
+      <c r="F22" s="11"/>
+    </row>
+    <row r="23" spans="2:6">
       <c r="B23" s="5"/>
       <c r="C23" s="3"/>
       <c r="D23" s="13"/>
       <c r="E23" s="11"/>
-    </row>
-    <row r="24" spans="2:5">
+      <c r="F23" s="11"/>
+    </row>
+    <row r="24" spans="2:6">
       <c r="B24" s="5"/>
       <c r="C24" s="3"/>
       <c r="D24" s="13"/>
       <c r="E24" s="11"/>
-    </row>
-    <row r="25" spans="2:5">
+      <c r="F24" s="11"/>
+    </row>
+    <row r="25" spans="2:6">
       <c r="B25" s="5"/>
       <c r="C25" s="3"/>
       <c r="D25" s="13"/>
       <c r="E25" s="11"/>
-    </row>
-    <row r="26" spans="2:5">
+      <c r="F25" s="11"/>
+    </row>
+    <row r="26" spans="2:6">
       <c r="B26" s="5"/>
       <c r="C26" s="3"/>
       <c r="D26" s="13"/>
       <c r="E26" s="11"/>
-    </row>
-    <row r="27" spans="2:5">
+      <c r="F26" s="11"/>
+    </row>
+    <row r="27" spans="2:6">
       <c r="B27" s="5"/>
       <c r="C27" s="3"/>
       <c r="D27" s="13"/>
       <c r="E27" s="11"/>
-    </row>
-    <row r="28" spans="2:5">
+      <c r="F27" s="11"/>
+    </row>
+    <row r="28" spans="2:6">
       <c r="B28" s="5"/>
       <c r="C28" s="3"/>
       <c r="D28" s="13"/>
       <c r="E28" s="11"/>
-    </row>
-    <row r="29" spans="2:5">
+      <c r="F28" s="11"/>
+    </row>
+    <row r="29" spans="2:6">
       <c r="B29" s="5"/>
       <c r="C29" s="3"/>
       <c r="D29" s="13"/>
       <c r="E29" s="11"/>
-    </row>
-    <row r="30" spans="2:5" ht="16" thickBot="1">
-      <c r="B30" s="6"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="12"/>
-    </row>
-    <row r="31" spans="2:5">
-      <c r="B31" s="1"/>
-      <c r="D31" s="2"/>
-    </row>
-    <row r="32" spans="2:5">
+      <c r="F29" s="11"/>
+    </row>
+    <row r="30" spans="2:6">
+      <c r="B30" s="5"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+    </row>
+    <row r="31" spans="2:6" ht="16" thickBot="1">
+      <c r="B31" s="6"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+    </row>
+    <row r="32" spans="2:6">
       <c r="B32" s="1"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B1:F1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Customer report section added.
</commit_message>
<xml_diff>
--- a/misc/Requests.xlsx
+++ b/misc/Requests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="29780" windowHeight="17620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="31300" windowHeight="18300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Requests" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>Priortiy</t>
   </si>
@@ -39,30 +39,18 @@
     <t xml:space="preserve">Make cosmetic changes to reports </t>
   </si>
   <si>
-    <t>Kian Notes</t>
-  </si>
-  <si>
     <t>Medium</t>
   </si>
   <si>
     <t>Create a 'Reports' section to declutter 'Products'</t>
   </si>
   <si>
-    <t>Merge 'add' functionality to products + customers section</t>
-  </si>
-  <si>
     <t>Products PO stock split per order + date</t>
   </si>
   <si>
-    <t>Alert when selecting customer for a new order</t>
-  </si>
-  <si>
     <t>Proforma customer alert</t>
   </si>
   <si>
-    <t>Use a template excel sheet for each report</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -88,6 +76,12 @@
   </si>
   <si>
     <t>1h</t>
+  </si>
+  <si>
+    <t>Create a customers report section</t>
+  </si>
+  <si>
+    <t>6h</t>
   </si>
 </sst>
 </file>
@@ -294,9 +288,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -341,13 +339,15 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="18">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
@@ -355,6 +355,8 @@
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -684,31 +686,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F34"/>
+  <dimension ref="B1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="58.33203125" customWidth="1"/>
     <col min="4" max="4" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="18">
+    <row r="1" spans="2:5" ht="18">
       <c r="B1" s="24" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-    </row>
-    <row r="2" spans="2:6" ht="16" thickBot="1"/>
-    <row r="3" spans="2:6" ht="19" thickBot="1">
+    </row>
+    <row r="2" spans="2:5" ht="16" thickBot="1"/>
+    <row r="3" spans="2:5" ht="19" thickBot="1">
       <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
@@ -719,62 +719,52 @@
         <v>2</v>
       </c>
       <c r="E3" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6">
-      <c r="B4" s="10" t="s">
+      <c r="C4" s="19" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>8</v>
       </c>
       <c r="D4" s="17">
         <v>42641</v>
       </c>
       <c r="E4" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>9</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6">
-      <c r="B5" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>12</v>
       </c>
       <c r="D5" s="17">
         <v>42650</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
       <c r="B6" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D6" s="17">
         <v>42653</v>
       </c>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6">
+      <c r="E6" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
       <c r="B7" s="20" t="s">
         <v>4</v>
       </c>
@@ -785,228 +775,207 @@
         <v>42660</v>
       </c>
       <c r="E7" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="22" t="s">
         <v>13</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6">
-      <c r="B8" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>17</v>
       </c>
       <c r="D8" s="23">
         <v>42660</v>
       </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18" t="s">
+      <c r="E8" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="22" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6">
-      <c r="B9" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>18</v>
       </c>
       <c r="D9" s="23">
         <v>42688</v>
       </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6">
+      <c r="E9" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
       <c r="B10" s="10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D10" s="23">
         <v>42692</v>
       </c>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6">
-      <c r="B11" s="5" t="s">
+      <c r="E10" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="17">
+        <v>42711</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-    </row>
-    <row r="12" spans="2:6">
-      <c r="B12" s="5"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="13"/>
+      <c r="C12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-    </row>
-    <row r="13" spans="2:6">
+    </row>
+    <row r="13" spans="2:5">
       <c r="B13" s="5"/>
       <c r="C13" s="3"/>
       <c r="D13" s="13"/>
       <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-    </row>
-    <row r="14" spans="2:6">
+    </row>
+    <row r="14" spans="2:5">
       <c r="B14" s="5"/>
       <c r="C14" s="3"/>
       <c r="D14" s="13"/>
       <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-    </row>
-    <row r="15" spans="2:6">
+    </row>
+    <row r="15" spans="2:5">
       <c r="B15" s="5"/>
       <c r="C15" s="3"/>
       <c r="D15" s="13"/>
       <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-    </row>
-    <row r="16" spans="2:6">
+    </row>
+    <row r="16" spans="2:5">
       <c r="B16" s="5"/>
       <c r="C16" s="3"/>
       <c r="D16" s="13"/>
       <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-    </row>
-    <row r="17" spans="2:6">
+    </row>
+    <row r="17" spans="2:5">
       <c r="B17" s="5"/>
       <c r="C17" s="3"/>
       <c r="D17" s="13"/>
       <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-    </row>
-    <row r="18" spans="2:6">
+    </row>
+    <row r="18" spans="2:5">
       <c r="B18" s="5"/>
       <c r="C18" s="3"/>
       <c r="D18" s="13"/>
       <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-    </row>
-    <row r="19" spans="2:6">
+    </row>
+    <row r="19" spans="2:5">
       <c r="B19" s="5"/>
       <c r="C19" s="3"/>
       <c r="D19" s="13"/>
       <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-    </row>
-    <row r="20" spans="2:6">
+    </row>
+    <row r="20" spans="2:5">
       <c r="B20" s="5"/>
       <c r="C20" s="3"/>
       <c r="D20" s="13"/>
       <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-    </row>
-    <row r="21" spans="2:6">
+    </row>
+    <row r="21" spans="2:5">
       <c r="B21" s="5"/>
       <c r="C21" s="3"/>
       <c r="D21" s="13"/>
       <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-    </row>
-    <row r="22" spans="2:6">
+    </row>
+    <row r="22" spans="2:5">
       <c r="B22" s="5"/>
       <c r="C22" s="3"/>
       <c r="D22" s="13"/>
       <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-    </row>
-    <row r="23" spans="2:6">
+    </row>
+    <row r="23" spans="2:5">
       <c r="B23" s="5"/>
       <c r="C23" s="3"/>
       <c r="D23" s="13"/>
       <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-    </row>
-    <row r="24" spans="2:6">
+    </row>
+    <row r="24" spans="2:5">
       <c r="B24" s="5"/>
       <c r="C24" s="3"/>
       <c r="D24" s="13"/>
       <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-    </row>
-    <row r="25" spans="2:6">
+    </row>
+    <row r="25" spans="2:5">
       <c r="B25" s="5"/>
       <c r="C25" s="3"/>
       <c r="D25" s="13"/>
       <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-    </row>
-    <row r="26" spans="2:6">
+    </row>
+    <row r="26" spans="2:5">
       <c r="B26" s="5"/>
       <c r="C26" s="3"/>
       <c r="D26" s="13"/>
       <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-    </row>
-    <row r="27" spans="2:6">
+    </row>
+    <row r="27" spans="2:5">
       <c r="B27" s="5"/>
       <c r="C27" s="3"/>
       <c r="D27" s="13"/>
       <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-    </row>
-    <row r="28" spans="2:6">
+    </row>
+    <row r="28" spans="2:5">
       <c r="B28" s="5"/>
       <c r="C28" s="3"/>
       <c r="D28" s="13"/>
       <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-    </row>
-    <row r="29" spans="2:6">
+    </row>
+    <row r="29" spans="2:5">
       <c r="B29" s="5"/>
       <c r="C29" s="3"/>
       <c r="D29" s="13"/>
       <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-    </row>
-    <row r="30" spans="2:6">
+    </row>
+    <row r="30" spans="2:5">
       <c r="B30" s="5"/>
       <c r="C30" s="3"/>
       <c r="D30" s="13"/>
       <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-    </row>
-    <row r="31" spans="2:6">
+    </row>
+    <row r="31" spans="2:5">
       <c r="B31" s="5"/>
       <c r="C31" s="3"/>
       <c r="D31" s="13"/>
       <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-    </row>
-    <row r="32" spans="2:6" ht="16" thickBot="1">
+    </row>
+    <row r="32" spans="2:5" ht="16" thickBot="1">
       <c r="B32" s="6"/>
       <c r="C32" s="4"/>
       <c r="D32" s="14"/>
       <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-    </row>
-    <row r="33" spans="2:5">
+    </row>
+    <row r="33" spans="2:4">
       <c r="B33" s="1"/>
       <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="2:5">
+    </row>
+    <row r="34" spans="2:4">
       <c r="B34" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B1:E1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>